<commit_message>
terminei a base de treinamento
</commit_message>
<xml_diff>
--- a/Trânsito.xlsx
+++ b/Trânsito.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnr\Desktop\Cdados dp\Projeto-1---Cdados-2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\OneDrive\Área de Trabalho\Insper\Cdados\Projeto-1---Cdados-2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C694BF7B-193F-4D94-BFC5-0128F406A37C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386EED50-C6F9-431A-8D09-933D41B4DB6A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="456">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1905,13 +1905,13 @@
       <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="122.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="122.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -3128,752 +3128,752 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>300</v>
       </c>
@@ -3885,60 +3885,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D151"/>
+  <dimension ref="A1:B151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="127.77734375" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="1" max="1" width="127.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="D1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>302</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>303</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>304</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>305</v>
       </c>
@@ -3946,7 +3934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>306</v>
       </c>
@@ -3954,7 +3942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>307</v>
       </c>
@@ -3962,7 +3950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>308</v>
       </c>
@@ -3970,7 +3958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>309</v>
       </c>
@@ -3978,7 +3966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>310</v>
       </c>
@@ -3986,7 +3974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>311</v>
       </c>
@@ -3994,7 +3982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>312</v>
       </c>
@@ -4002,7 +3990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>313</v>
       </c>
@@ -4010,7 +3998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>314</v>
       </c>
@@ -4018,7 +4006,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>315</v>
       </c>
@@ -4026,7 +4014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>316</v>
       </c>
@@ -4034,7 +4022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>317</v>
       </c>
@@ -4042,7 +4030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>318</v>
       </c>
@@ -4050,7 +4038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>319</v>
       </c>
@@ -4058,7 +4046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>320</v>
       </c>
@@ -4066,7 +4054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>321</v>
       </c>
@@ -4074,7 +4062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>322</v>
       </c>
@@ -4082,7 +4070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>323</v>
       </c>
@@ -4090,7 +4078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>324</v>
       </c>
@@ -4098,7 +4086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>325</v>
       </c>
@@ -4106,7 +4094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>326</v>
       </c>
@@ -4114,7 +4102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>327</v>
       </c>
@@ -4122,7 +4110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>328</v>
       </c>
@@ -4130,7 +4118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>329</v>
       </c>
@@ -4138,7 +4126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>330</v>
       </c>
@@ -4146,7 +4134,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>331</v>
       </c>
@@ -4154,7 +4142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>332</v>
       </c>
@@ -4162,7 +4150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>333</v>
       </c>
@@ -4170,7 +4158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>334</v>
       </c>
@@ -4178,7 +4166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>335</v>
       </c>
@@ -4186,7 +4174,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>336</v>
       </c>
@@ -4194,7 +4182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>337</v>
       </c>
@@ -4202,7 +4190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>338</v>
       </c>
@@ -4210,7 +4198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>339</v>
       </c>
@@ -4218,7 +4206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>340</v>
       </c>
@@ -4226,7 +4214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>341</v>
       </c>
@@ -4234,7 +4222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>342</v>
       </c>
@@ -4242,7 +4230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>343</v>
       </c>
@@ -4250,7 +4238,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>344</v>
       </c>
@@ -4258,7 +4246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>345</v>
       </c>
@@ -4266,7 +4254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>346</v>
       </c>
@@ -4274,7 +4262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>347</v>
       </c>
@@ -4282,7 +4270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>348</v>
       </c>
@@ -4290,7 +4278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>349</v>
       </c>
@@ -4298,7 +4286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>350</v>
       </c>
@@ -4306,7 +4294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>351</v>
       </c>
@@ -4314,7 +4302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>352</v>
       </c>
@@ -4322,7 +4310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>353</v>
       </c>
@@ -4330,7 +4318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>354</v>
       </c>
@@ -4338,7 +4326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>355</v>
       </c>
@@ -4346,7 +4334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>356</v>
       </c>
@@ -4354,7 +4342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>357</v>
       </c>
@@ -4362,7 +4350,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>358</v>
       </c>
@@ -4370,7 +4358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>359</v>
       </c>
@@ -4378,7 +4366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>360</v>
       </c>
@@ -4386,7 +4374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>361</v>
       </c>
@@ -4394,7 +4382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>362</v>
       </c>
@@ -4402,7 +4390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>363</v>
       </c>
@@ -4410,7 +4398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>364</v>
       </c>
@@ -4418,7 +4406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>365</v>
       </c>
@@ -4426,7 +4414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>366</v>
       </c>
@@ -4434,7 +4422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>367</v>
       </c>
@@ -4442,7 +4430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>368</v>
       </c>
@@ -4450,7 +4438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>369</v>
       </c>
@@ -4458,7 +4446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>370</v>
       </c>
@@ -4466,7 +4454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>371</v>
       </c>
@@ -4474,7 +4462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>372</v>
       </c>
@@ -4482,7 +4470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>373</v>
       </c>
@@ -4490,7 +4478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>374</v>
       </c>
@@ -4498,7 +4486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>375</v>
       </c>
@@ -4506,384 +4494,612 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B145">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B148">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>451</v>
+      </c>
+      <c r="B151">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Até parte 3 do guia
</commit_message>
<xml_diff>
--- a/Trânsito.xlsx
+++ b/Trânsito.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\OneDrive\Área de Trabalho\Insper\Cdados\Projeto-1---Cdados-2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnr\Desktop\Cdados dp\Projeto-1---Cdados-2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813AA7DA-39D6-4C7A-B5C6-CED07E8C1680}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C293039-5226-4F67-A94F-3F16E876A650}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -1892,18 +1892,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="122.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="122.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>177</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>180</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>183</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>185</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>188</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>190</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>193</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>195</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>197</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>198</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>200</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>202</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>222</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>223</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>225</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>226</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>227</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>228</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>229</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>230</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>231</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>232</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>233</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>234</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>235</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>236</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>237</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>238</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>239</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>240</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>241</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>242</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>243</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>244</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>245</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>246</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>247</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>248</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>250</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>251</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>252</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>253</v>
       </c>
@@ -3935,7 +3935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>254</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>256</v>
       </c>
@@ -3959,7 +3959,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>257</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>258</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>259</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>260</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>261</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>263</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>264</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>265</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>266</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>267</v>
       </c>
@@ -4047,7 +4047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>268</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>269</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>270</v>
       </c>
@@ -4071,7 +4071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>271</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>272</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>273</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>274</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>275</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>276</v>
       </c>
@@ -4119,7 +4119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>277</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>278</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>279</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>280</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>281</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>282</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>283</v>
       </c>
@@ -4175,7 +4175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>284</v>
       </c>
@@ -4183,7 +4183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>285</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>286</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>287</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>288</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>289</v>
       </c>
@@ -4223,7 +4223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>290</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>291</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>292</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>293</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>294</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>295</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>296</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>297</v>
       </c>
@@ -4287,7 +4287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>298</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>299</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>300</v>
       </c>
@@ -4320,17 +4320,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A127" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="127.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="127.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>301</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>302</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>303</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>304</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>305</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>306</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>307</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>308</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>309</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>310</v>
       </c>
@@ -4410,7 +4410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>311</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>312</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>313</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>314</v>
       </c>
@@ -4442,7 +4442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>315</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>316</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>317</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>318</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>319</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>320</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>321</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>322</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>323</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>324</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>325</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>326</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>327</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>328</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>329</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>330</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>331</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>332</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>333</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>334</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>335</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>336</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>337</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>338</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>339</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>340</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>341</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>342</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>343</v>
       </c>
@@ -4674,7 +4674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>344</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>345</v>
       </c>
@@ -4690,7 +4690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>346</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>347</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>348</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>349</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>350</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>351</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>352</v>
       </c>
@@ -4746,7 +4746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>353</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>354</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>355</v>
       </c>
@@ -4770,7 +4770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>356</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>357</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>358</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>359</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>360</v>
       </c>
@@ -4810,7 +4810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>361</v>
       </c>
@@ -4818,7 +4818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>362</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>363</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>364</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>365</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>366</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>367</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>368</v>
       </c>
@@ -4874,7 +4874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>369</v>
       </c>
@@ -4882,7 +4882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>370</v>
       </c>
@@ -4890,7 +4890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>371</v>
       </c>
@@ -4898,7 +4898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>372</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>373</v>
       </c>
@@ -4914,7 +4914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>374</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>375</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>376</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>377</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>378</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>379</v>
       </c>
@@ -4962,7 +4962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>380</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>381</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>382</v>
       </c>
@@ -4986,7 +4986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>383</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>384</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>385</v>
       </c>
@@ -5010,7 +5010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>386</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>387</v>
       </c>
@@ -5026,7 +5026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>388</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>389</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>390</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>391</v>
       </c>
@@ -5058,7 +5058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>392</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>393</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>394</v>
       </c>
@@ -5082,7 +5082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>395</v>
       </c>
@@ -5090,7 +5090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>396</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>397</v>
       </c>
@@ -5106,7 +5106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>398</v>
       </c>
@@ -5114,7 +5114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>399</v>
       </c>
@@ -5122,7 +5122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>400</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>401</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>402</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>403</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>404</v>
       </c>
@@ -5162,7 +5162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>405</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>406</v>
       </c>
@@ -5178,7 +5178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>407</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>408</v>
       </c>
@@ -5194,7 +5194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>409</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>410</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>411</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>412</v>
       </c>
@@ -5226,7 +5226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>413</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>414</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>415</v>
       </c>
@@ -5250,7 +5250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>416</v>
       </c>
@@ -5258,7 +5258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>417</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>418</v>
       </c>
@@ -5274,7 +5274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>419</v>
       </c>
@@ -5282,7 +5282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>420</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>421</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>422</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>423</v>
       </c>
@@ -5314,7 +5314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>424</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>425</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>426</v>
       </c>
@@ -5338,7 +5338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>427</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>428</v>
       </c>
@@ -5354,7 +5354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>429</v>
       </c>
@@ -5362,7 +5362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>430</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>431</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>432</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>433</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>434</v>
       </c>
@@ -5402,7 +5402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>435</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>436</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>437</v>
       </c>
@@ -5426,7 +5426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>438</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>439</v>
       </c>
@@ -5442,7 +5442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>440</v>
       </c>
@@ -5450,7 +5450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>441</v>
       </c>
@@ -5458,7 +5458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>442</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>443</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>444</v>
       </c>
@@ -5482,7 +5482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>445</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>446</v>
       </c>
@@ -5498,7 +5498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>447</v>
       </c>
@@ -5506,7 +5506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>448</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>449</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>450</v>
       </c>
@@ -5530,7 +5530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>451</v>
       </c>

</xml_diff>